<commit_message>
memory imporvements -> colortable
</commit_message>
<xml_diff>
--- a/tools/frame_builder.xlsx
+++ b/tools/frame_builder.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelochsendorf/Desktop/WeatherFrame/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marcel\Desktop\WeatherFrame\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="440" windowWidth="18140" windowHeight="14540"/>
+    <workbookView xWindow="3675" yWindow="435" windowWidth="18135" windowHeight="14535"/>
   </bookViews>
   <sheets>
     <sheet name="FRAME_BUILDER" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -26,8 +26,16 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>FRAME COUNT</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -60,7 +68,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -79,6 +87,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -94,7 +108,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -123,49 +137,16 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF9522C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF68F442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF659CEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -184,6 +165,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,19 +472,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:A19"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="5.1640625" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.125" defaultRowHeight="22.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.1640625" style="3"/>
-    <col min="3" max="3" width="6.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="5.1640625" style="3"/>
+    <col min="1" max="1" width="6.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.125" style="3"/>
+    <col min="3" max="3" width="6.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="5.125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -545,7 +529,7 @@
       <c r="AP1" s="4"/>
       <c r="AQ1" s="4"/>
     </row>
-    <row r="2" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4">
         <v>0</v>
@@ -606,7 +590,7 @@
       <c r="AP2" s="4"/>
       <c r="AQ2" s="4"/>
     </row>
-    <row r="3" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="4">
         <v>0</v>
@@ -667,7 +651,7 @@
       <c r="AP3" s="4"/>
       <c r="AQ3" s="4"/>
     </row>
-    <row r="4" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4">
         <v>0</v>
@@ -728,7 +712,7 @@
       <c r="AP4" s="4"/>
       <c r="AQ4" s="4"/>
     </row>
-    <row r="5" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="4">
         <v>0</v>
@@ -789,7 +773,7 @@
       <c r="AP5" s="4"/>
       <c r="AQ5" s="4"/>
     </row>
-    <row r="6" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="4">
         <v>0</v>
@@ -850,7 +834,7 @@
       <c r="AP6" s="4"/>
       <c r="AQ6" s="4"/>
     </row>
-    <row r="7" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="4">
         <v>0</v>
@@ -911,7 +895,7 @@
       <c r="AP7" s="4"/>
       <c r="AQ7" s="4"/>
     </row>
-    <row r="8" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="4">
         <v>0</v>
@@ -972,7 +956,7 @@
       <c r="AP8" s="4"/>
       <c r="AQ8" s="4"/>
     </row>
-    <row r="9" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="4">
         <v>0</v>
@@ -1033,7 +1017,7 @@
       <c r="AP9" s="4"/>
       <c r="AQ9" s="4"/>
     </row>
-    <row r="10" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1078,7 +1062,7 @@
       <c r="AP10" s="4"/>
       <c r="AQ10" s="4"/>
     </row>
-    <row r="11" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1123,7 +1107,7 @@
       <c r="AP11" s="4"/>
       <c r="AQ11" s="4"/>
     </row>
-    <row r="12" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="str">
         <f>""&amp;B2&amp;","&amp;C2&amp;","&amp;D2&amp;","&amp;E2&amp;","&amp;F2&amp;","&amp;G2&amp;","&amp;H2&amp;","&amp;I2&amp;""</f>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1171,7 +1155,7 @@
       <c r="AP12" s="4"/>
       <c r="AQ12" s="4"/>
     </row>
-    <row r="13" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="str">
         <f t="shared" ref="A13:A19" si="0">""&amp;B3&amp;","&amp;C3&amp;","&amp;D3&amp;","&amp;E3&amp;","&amp;F3&amp;","&amp;G3&amp;","&amp;H3&amp;","&amp;I3&amp;""</f>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1219,7 +1203,7 @@
       <c r="AP13" s="4"/>
       <c r="AQ13" s="4"/>
     </row>
-    <row r="14" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1267,7 +1251,7 @@
       <c r="AP14" s="4"/>
       <c r="AQ14" s="4"/>
     </row>
-    <row r="15" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1315,7 +1299,7 @@
       <c r="AP15" s="4"/>
       <c r="AQ15" s="4"/>
     </row>
-    <row r="16" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1363,7 +1347,7 @@
       <c r="AP16" s="4"/>
       <c r="AQ16" s="4"/>
     </row>
-    <row r="17" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1411,7 +1395,7 @@
       <c r="AP17" s="4"/>
       <c r="AQ17" s="4"/>
     </row>
-    <row r="18" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1459,7 +1443,7 @@
       <c r="AP18" s="4"/>
       <c r="AQ18" s="4"/>
     </row>
-    <row r="19" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="str">
         <f t="shared" si="0"/>
         <v>0,0,0,0,0,0,0,0</v>
@@ -1507,10 +1491,14 @@
       <c r="AP19" s="4"/>
       <c r="AQ19" s="4"/>
     </row>
-    <row r="20" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
+    <row r="20" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
+      <c r="C20" s="10">
+        <v>4</v>
+      </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1552,7 +1540,7 @@
       <c r="AP20" s="4"/>
       <c r="AQ20" s="4"/>
     </row>
-    <row r="21" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1597,53 +1585,44 @@
       <c r="AP21" s="4"/>
       <c r="AQ21" s="4"/>
     </row>
-    <row r="24" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="6" t="str">
-        <f xml:space="preserve"> "const frame_data [" &amp; E13 &amp;"][8][8] = {"</f>
-        <v>const frame_data [][8][8] = {</v>
+    <row r="24" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="str">
+        <f xml:space="preserve"> "const frame_data [" &amp; C20 &amp;"][8][8] = {"</f>
+        <v>const frame_data [4][8][8] = {</v>
       </c>
       <c r="G24" s="6" t="str">
         <f xml:space="preserve"> "{"&amp; C14 &amp;","&amp;C15 &amp;","&amp;C16 &amp;","&amp;C17&amp;","&amp;C18 &amp;","&amp;C19 &amp;","&amp;C20 &amp;","&amp;C21 &amp;"," &amp;"},"</f>
-        <v>{,,,,,,,,},</v>
-      </c>
-    </row>
-    <row r="25" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>{,,,,,,4,,},</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G25" s="6" t="str">
         <f xml:space="preserve"> "{"&amp; N14 &amp;","&amp;N15 &amp;","&amp;N16 &amp;","&amp;N17&amp;","&amp;N18 &amp;","&amp;N19 &amp;","&amp;N20 &amp;","&amp;N21 &amp;"," &amp;"},"</f>
         <v>{,,,,,,,,},</v>
       </c>
     </row>
-    <row r="26" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G26" s="6" t="str">
         <f xml:space="preserve"> "{"&amp; Y14 &amp;","&amp;Y15 &amp;","&amp;Y16 &amp;","&amp;Y17&amp;","&amp;Y18 &amp;","&amp;Y19 &amp;","&amp;Y20 &amp;","&amp;Y21 &amp;"," &amp;"},"</f>
         <v>{,,,,,,,,},</v>
       </c>
     </row>
-    <row r="27" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G27" s="6" t="str">
         <f xml:space="preserve"> "{"&amp; AJ14 &amp;","&amp;AJ15 &amp;","&amp;AJ16 &amp;","&amp;AJ17&amp;","&amp;AJ18 &amp;","&amp;AJ19 &amp;","&amp;AJ20 &amp;","&amp;AJ21 &amp;"," &amp;"},"</f>
         <v>{,,,,,,,,},</v>
       </c>
     </row>
-    <row r="28" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E28" s="3" t="str">
         <f xml:space="preserve"> "}"</f>
         <v>}</v>
       </c>
     </row>
-    <row r="29" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="6" t="str">
-        <f xml:space="preserve"> "const std::string animation_name = " &amp; E12 &amp;";"</f>
-        <v>const std::string animation_name = ;</v>
-      </c>
-    </row>
-    <row r="30" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="str">
-        <f>"const int"</f>
-        <v>const int</v>
-      </c>
-    </row>
-    <row r="34" spans="7:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:43" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+    </row>
+    <row r="34" spans="7:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G34" s="6"/>
     </row>
   </sheetData>

</xml_diff>